<commit_message>
Update input files to match General Network Code.
In past versions of this code, the metric_input.xlsx files listed first path survival and then path probabilities for each season, this was different than the setup in the Generalized Network Code, making the two incompatible. This update fixes this problem by correctly ordering the metric_input files and changing the GR.R code to read in the data in the correct locations. This means the code is not backward compatible so all old input files must be reordered before using the latest version.
</commit_message>
<xml_diff>
--- a/Pulliam_Metapopulation/metric_inputs_adults.xlsx
+++ b/Pulliam_Metapopulation/metric_inputs_adults.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christine\Google Drive\research\NIMBioS\PerturbationCrAnalysisPaperME\RCode\GmetricCode_for_GmetricPaper\Pulliam_Metapop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samplec\Google Drive\research\NIMBioS\PerturbationCrAnalysisPaper\RCode\Gmetric-1.1-July.23.19\Pulliam_Metapopulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB1A8FD-8042-44FF-B156-55AD4D3EB314}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16387" windowHeight="8193" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22515" windowHeight="10905" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Breeding" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -89,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -218,15 +217,6 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -252,6 +242,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,224 +565,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" style="4"/>
-    <col min="4" max="4" width="21.5546875"/>
-    <col min="5" max="5" width="21.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.71875"/>
+    <col min="2" max="2" width="12.5" style="1"/>
+    <col min="4" max="4" width="21.5"/>
+    <col min="5" max="5" width="21.25" customWidth="1"/>
+    <col min="6" max="6" width="17.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="94" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>40</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>1.2</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <v>0</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <v>60</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <f>E15</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="18">
         <v>0</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="14"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="15">
-        <v>1</v>
-      </c>
-      <c r="D7" s="23">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12">
-        <v>1</v>
-      </c>
-      <c r="C8" s="15">
-        <v>1</v>
-      </c>
-      <c r="D8" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1"/>
-      <c r="B9" s="19">
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12">
+        <f>F8/C3*(D3-1)</f>
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="D8" s="20">
+        <f>1-C8</f>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="16">
         <v>2</v>
       </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="25"/>
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="15">
-        <v>1</v>
-      </c>
-      <c r="D12" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="12">
-        <v>1</v>
-      </c>
-      <c r="C13" s="15">
-        <f>F13/C3*(D3-1)</f>
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="D13" s="23">
-        <f>1-C13</f>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1"/>
-      <c r="B14" s="19">
-        <v>2</v>
-      </c>
-      <c r="C14" s="20">
+      <c r="C9" s="17">
         <v>0</v>
       </c>
-      <c r="D14" s="24">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="D9" s="21">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <f>C3*D3</f>
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="16">
+        <v>2</v>
+      </c>
+      <c r="C14" s="17">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15">
-        <f>(100-E14)/C4</f>
+        <f>(100-E9)/C4</f>
         <v>0.8666666666666667</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>